<commit_message>
v0.0.21 fix Immunization vaccinecode bindings
</commit_message>
<xml_diff>
--- a/StructureDefinition-Vaccine-Certificate-Immunization.xlsx
+++ b/StructureDefinition-Vaccine-Certificate-Immunization.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2269" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2270" uniqueCount="389">
   <si>
     <t>Path</t>
   </si>
@@ -451,7 +451,13 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/uv/smarthealthcards-vaccination/ValueSet/vaccine-credential-vaccine-value-set</t>
+    <t>example</t>
+  </si>
+  <si>
+    <t>The code for vaccine product administered.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/vaccine-code</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -906,9 +912,6 @@
   </si>
   <si>
     <t>Reasons why the vaccine was administered.</t>
-  </si>
-  <si>
-    <t>example</t>
   </si>
   <si>
     <t>The reason why a vaccine was administered.</t>
@@ -2963,11 +2966,13 @@
         <v>41</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="X14" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="X14" t="s" s="2">
+        <v>140</v>
+      </c>
       <c r="Y14" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>41</v>
@@ -3000,24 +3005,24 @@
         <v>64</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3040,13 +3045,13 @@
         <v>52</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -3097,7 +3102,7 @@
         <v>41</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>51</v>
@@ -3112,16 +3117,16 @@
         <v>64</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AN15" t="s" s="2">
         <v>41</v>
@@ -3129,7 +3134,7 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3152,13 +3157,13 @@
         <v>41</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -3209,7 +3214,7 @@
         <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>42</v>
@@ -3224,16 +3229,16 @@
         <v>64</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AN16" t="s" s="2">
         <v>41</v>
@@ -3241,7 +3246,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3264,16 +3269,16 @@
         <v>52</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -3311,17 +3316,17 @@
         <v>41</v>
       </c>
       <c r="AA17" t="s" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AB17" s="2"/>
       <c r="AC17" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD17" t="s" s="2">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>51</v>
@@ -3336,24 +3341,24 @@
         <v>64</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3376,13 +3381,13 @@
         <v>41</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3433,7 +3438,7 @@
         <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>42</v>
@@ -3454,10 +3459,10 @@
         <v>41</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>41</v>
@@ -3465,7 +3470,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3488,16 +3493,16 @@
         <v>52</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3547,7 +3552,7 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>42</v>
@@ -3565,13 +3570,13 @@
         <v>41</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>41</v>
@@ -3579,7 +3584,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3605,13 +3610,13 @@
         <v>128</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3641,7 +3646,7 @@
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>41</v>
@@ -3659,7 +3664,7 @@
         <v>41</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>42</v>
@@ -3677,13 +3682,13 @@
         <v>41</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>41</v>
@@ -3691,7 +3696,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3714,13 +3719,13 @@
         <v>41</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3771,7 +3776,7 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>42</v>
@@ -3786,16 +3791,16 @@
         <v>64</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>41</v>
@@ -3803,7 +3808,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3826,13 +3831,13 @@
         <v>41</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3883,7 +3888,7 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>42</v>
@@ -3901,21 +3906,21 @@
         <v>41</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3941,10 +3946,10 @@
         <v>53</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -3995,7 +4000,7 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>42</v>
@@ -4007,27 +4012,27 @@
         <v>41</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4050,13 +4055,13 @@
         <v>41</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -4107,7 +4112,7 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>42</v>
@@ -4125,10 +4130,10 @@
         <v>41</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>41</v>
@@ -4139,7 +4144,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4165,10 +4170,10 @@
         <v>128</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -4199,7 +4204,7 @@
       </c>
       <c r="X25" s="2"/>
       <c r="Y25" t="s" s="2">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>41</v>
@@ -4217,7 +4222,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>42</v>
@@ -4235,21 +4240,21 @@
         <v>41</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4275,10 +4280,10 @@
         <v>128</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -4309,7 +4314,7 @@
       </c>
       <c r="X26" s="2"/>
       <c r="Y26" t="s" s="2">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>41</v>
@@ -4327,7 +4332,7 @@
         <v>41</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>42</v>
@@ -4345,21 +4350,21 @@
         <v>41</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4382,13 +4387,13 @@
         <v>41</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -4439,7 +4444,7 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>42</v>
@@ -4457,10 +4462,10 @@
         <v>41</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>41</v>
@@ -4471,7 +4476,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4494,13 +4499,13 @@
         <v>52</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4551,7 +4556,7 @@
         <v>41</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>42</v>
@@ -4566,13 +4571,13 @@
         <v>64</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>41</v>
@@ -4583,7 +4588,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4609,10 +4614,10 @@
         <v>53</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4663,7 +4668,7 @@
         <v>41</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>42</v>
@@ -4684,7 +4689,7 @@
         <v>41</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>41</v>
@@ -4695,7 +4700,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4724,7 +4729,7 @@
         <v>99</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M30" t="s" s="2">
         <v>101</v>
@@ -4777,7 +4782,7 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>42</v>
@@ -4798,7 +4803,7 @@
         <v>41</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>41</v>
@@ -4809,11 +4814,11 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -4835,10 +4840,10 @@
         <v>98</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="M31" t="s" s="2">
         <v>101</v>
@@ -4893,7 +4898,7 @@
         <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>42</v>
@@ -4925,7 +4930,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4951,10 +4956,10 @@
         <v>128</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4984,10 +4989,10 @@
         <v>132</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>41</v>
@@ -5005,7 +5010,7 @@
         <v>41</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>42</v>
@@ -5020,13 +5025,13 @@
         <v>64</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>41</v>
@@ -5037,7 +5042,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5060,16 +5065,16 @@
         <v>52</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
@@ -5119,7 +5124,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>51</v>
@@ -5134,16 +5139,16 @@
         <v>64</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>41</v>
@@ -5151,7 +5156,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5174,13 +5179,13 @@
         <v>52</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5231,7 +5236,7 @@
         <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>42</v>
@@ -5246,13 +5251,13 @@
         <v>64</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>41</v>
@@ -5263,7 +5268,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5289,10 +5294,10 @@
         <v>128</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5319,13 +5324,13 @@
         <v>41</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>286</v>
+        <v>139</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>41</v>
@@ -5343,7 +5348,7 @@
         <v>41</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
@@ -5358,13 +5363,13 @@
         <v>64</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>41</v>
@@ -5375,7 +5380,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5398,13 +5403,13 @@
         <v>41</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5455,7 +5460,7 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>42</v>
@@ -5470,7 +5475,7 @@
         <v>64</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>41</v>
@@ -5487,7 +5492,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5510,23 +5515,23 @@
         <v>52</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P37" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="Q37" t="s" s="2">
         <v>41</v>
@@ -5571,7 +5576,7 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>42</v>
@@ -5583,13 +5588,13 @@
         <v>41</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>95</v>
@@ -5603,7 +5608,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5629,10 +5634,10 @@
         <v>128</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5659,13 +5664,13 @@
         <v>41</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>286</v>
+        <v>139</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>41</v>
@@ -5683,7 +5688,7 @@
         <v>41</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>42</v>
@@ -5715,7 +5720,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5738,13 +5743,13 @@
         <v>41</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5795,7 +5800,7 @@
         <v>41</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>42</v>
@@ -5807,7 +5812,7 @@
         <v>41</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>41</v>
@@ -5827,7 +5832,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5853,10 +5858,10 @@
         <v>53</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5907,7 +5912,7 @@
         <v>41</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>42</v>
@@ -5928,7 +5933,7 @@
         <v>41</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>41</v>
@@ -5939,7 +5944,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5968,7 +5973,7 @@
         <v>99</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M41" t="s" s="2">
         <v>101</v>
@@ -6021,7 +6026,7 @@
         <v>41</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>42</v>
@@ -6042,7 +6047,7 @@
         <v>41</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>41</v>
@@ -6053,11 +6058,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6079,10 +6084,10 @@
         <v>98</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>101</v>
@@ -6137,7 +6142,7 @@
         <v>41</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>42</v>
@@ -6169,7 +6174,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6195,10 +6200,10 @@
         <v>53</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6249,7 +6254,7 @@
         <v>41</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>42</v>
@@ -6267,7 +6272,7 @@
         <v>41</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>95</v>
@@ -6281,7 +6286,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6307,10 +6312,10 @@
         <v>66</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6361,7 +6366,7 @@
         <v>41</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>42</v>
@@ -6393,7 +6398,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6416,13 +6421,13 @@
         <v>41</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6473,7 +6478,7 @@
         <v>41</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>42</v>
@@ -6491,7 +6496,7 @@
         <v>41</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>95</v>
@@ -6505,7 +6510,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6528,13 +6533,13 @@
         <v>41</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6585,7 +6590,7 @@
         <v>41</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>42</v>
@@ -6603,7 +6608,7 @@
         <v>41</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>95</v>
@@ -6617,7 +6622,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6643,10 +6648,10 @@
         <v>128</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6673,13 +6678,13 @@
         <v>41</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>286</v>
+        <v>139</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>41</v>
@@ -6697,7 +6702,7 @@
         <v>41</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>42</v>
@@ -6715,7 +6720,7 @@
         <v>41</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>95</v>
@@ -6729,7 +6734,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6755,10 +6760,10 @@
         <v>128</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6789,7 +6794,7 @@
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>41</v>
@@ -6807,7 +6812,7 @@
         <v>41</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>42</v>
@@ -6839,7 +6844,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6862,16 +6867,16 @@
         <v>41</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6921,7 +6926,7 @@
         <v>41</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>42</v>
@@ -6939,10 +6944,10 @@
         <v>41</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>41</v>
@@ -6953,7 +6958,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6979,10 +6984,10 @@
         <v>53</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -7033,7 +7038,7 @@
         <v>41</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>42</v>
@@ -7054,7 +7059,7 @@
         <v>41</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>41</v>
@@ -7065,7 +7070,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7094,7 +7099,7 @@
         <v>99</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M51" t="s" s="2">
         <v>101</v>
@@ -7147,7 +7152,7 @@
         <v>41</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>42</v>
@@ -7168,7 +7173,7 @@
         <v>41</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>41</v>
@@ -7179,11 +7184,11 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7205,10 +7210,10 @@
         <v>98</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>101</v>
@@ -7263,7 +7268,7 @@
         <v>41</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>42</v>
@@ -7295,7 +7300,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7318,13 +7323,13 @@
         <v>41</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7375,7 +7380,7 @@
         <v>41</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>42</v>
@@ -7393,10 +7398,10 @@
         <v>41</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>41</v>
@@ -7407,7 +7412,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7430,13 +7435,13 @@
         <v>41</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7487,7 +7492,7 @@
         <v>41</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>42</v>
@@ -7505,10 +7510,10 @@
         <v>41</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>41</v>
@@ -7519,7 +7524,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7542,13 +7547,13 @@
         <v>41</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7599,7 +7604,7 @@
         <v>41</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>42</v>
@@ -7617,10 +7622,10 @@
         <v>41</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>41</v>
@@ -7631,7 +7636,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7654,13 +7659,13 @@
         <v>41</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7711,7 +7716,7 @@
         <v>41</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>42</v>
@@ -7743,7 +7748,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7769,10 +7774,10 @@
         <v>53</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7823,7 +7828,7 @@
         <v>41</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>42</v>
@@ -7844,7 +7849,7 @@
         <v>41</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>41</v>
@@ -7855,7 +7860,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7884,7 +7889,7 @@
         <v>99</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M58" t="s" s="2">
         <v>101</v>
@@ -7937,7 +7942,7 @@
         <v>41</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>42</v>
@@ -7958,7 +7963,7 @@
         <v>41</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>41</v>
@@ -7969,11 +7974,11 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
@@ -7995,10 +8000,10 @@
         <v>98</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="M59" t="s" s="2">
         <v>101</v>
@@ -8053,7 +8058,7 @@
         <v>41</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>42</v>
@@ -8085,7 +8090,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8111,10 +8116,10 @@
         <v>53</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -8165,7 +8170,7 @@
         <v>41</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8197,7 +8202,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8220,13 +8225,13 @@
         <v>41</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8277,7 +8282,7 @@
         <v>41</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>42</v>
@@ -8309,7 +8314,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8335,10 +8340,10 @@
         <v>128</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8365,13 +8370,13 @@
         <v>41</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>286</v>
+        <v>139</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>41</v>
@@ -8389,7 +8394,7 @@
         <v>41</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>42</v>
@@ -8421,7 +8426,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8444,16 +8449,16 @@
         <v>41</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8503,7 +8508,7 @@
         <v>41</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>51</v>
@@ -8535,7 +8540,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8558,16 +8563,16 @@
         <v>41</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8617,7 +8622,7 @@
         <v>41</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>42</v>

</xml_diff>